<commit_message>
update function for ExcelTool
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\woodwhales-common\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\woodwhales\woodwhales-common\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F161626-9F37-4572-A3EF-857960B35DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3ECC7-EC93-49BB-B693-7F791975F127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="1260" windowWidth="22275" windowHeight="13005" xr2:uid="{0487492B-EC4D-43B5-A44D-ED4F1AE7B453}"/>
+    <workbookView xWindow="1935" yWindow="2820" windowWidth="25095" windowHeight="13575" xr2:uid="{0487492B-EC4D-43B5-A44D-ED4F1AE7B453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>性别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>男</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,6 +89,10 @@
   </si>
   <si>
     <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gender</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +466,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -484,30 +484,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>13112344321</v>
@@ -519,18 +519,18 @@
         <v>44406.375</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>13112344322</v>
@@ -542,18 +542,18 @@
         <v>44405.375</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>13112344323</v>
@@ -565,7 +565,7 @@
         <v>44404.375</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function for ExcelTool: set default value when parse data
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\#woodwhales\new\woodwhales-common\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F84860D-E0A6-4AC9-B35B-34D4F3565D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB470037-B7B9-4FAE-8FF3-A37158B35066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="27910" windowHeight="15950" xr2:uid="{0487492B-EC4D-43B5-A44D-ED4F1AE7B453}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0487492B-EC4D-43B5-A44D-ED4F1AE7B453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +101,10 @@
   </si>
   <si>
     <t>{"address": "北京","tag": "常住地"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDECB5B-E943-4717-BC7A-C921AE7474BE}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -485,7 +489,7 @@
     <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +514,11 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -533,11 +540,11 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -559,8 +566,11 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -581,6 +591,9 @@
       </c>
       <c r="G4" t="s">
         <v>11</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>